<commit_message>
feat: Add a digit recognition system using Euclidean distance, along with reference patterns, input examples, frequency matrices, and detailed documentation
</commit_message>
<xml_diff>
--- a/DetectorNumeros/frecuencias/matrices_cuatro_10.xlsx
+++ b/DetectorNumeros/frecuencias/matrices_cuatro_10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guere\Documents\Tec\7mo\IA\Programas 2do Parcial\DetectorNumeros\frecuencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Escuela\7mo_semestre\Inteligencia Artificial\CodigosRepo\Programas-2do-Parcial\DetectorNumeros\frecuencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D09997-1B5A-49EE-AB97-33C184405CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E47FE6-2424-4BF9-A13C-FA17DE7C95A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="10" xr2:uid="{E6A55DB8-9F2F-4D1A-93E6-192E366E17F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6A55DB8-9F2F-4D1A-93E6-192E366E17F4}"/>
   </bookViews>
   <sheets>
     <sheet name="matrix1" sheetId="1" r:id="rId1"/>
@@ -414,16 +414,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F058C95-388E-41C6-BA33-5E76BAC0C5A5}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -681,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2838,18 +2838,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2102CB76-92FC-4745-A3F1-B818B8803709}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+      <selection activeCell="A26" sqref="A26:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -5082,6 +5082,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>
@@ -5094,16 +5266,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E264A3E5-B8B9-46F7-8481-EA9A839DCEDF}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(matrix1:matrix10!A1)</f>
         <v>0</v>
@@ -5217,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM(matrix1:matrix10!A2)</f>
         <v>0</v>
@@ -5331,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>SUM(matrix1:matrix10!A3)</f>
         <v>0</v>
@@ -5445,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>SUM(matrix1:matrix10!A4)</f>
         <v>0</v>
@@ -5559,7 +5731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>SUM(matrix1:matrix10!A5)</f>
         <v>0</v>
@@ -5673,7 +5845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>SUM(matrix1:matrix10!A6)</f>
         <v>0</v>
@@ -5787,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>SUM(matrix1:matrix10!A7)</f>
         <v>0</v>
@@ -5901,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>SUM(matrix1:matrix10!A8)</f>
         <v>0</v>
@@ -6015,7 +6187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>SUM(matrix1:matrix10!A9)</f>
         <v>0</v>
@@ -6129,7 +6301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>SUM(matrix1:matrix10!A10)</f>
         <v>0</v>
@@ -6243,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>SUM(matrix1:matrix10!A11)</f>
         <v>0</v>
@@ -6357,7 +6529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>SUM(matrix1:matrix10!A12)</f>
         <v>0</v>
@@ -6471,7 +6643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>SUM(matrix1:matrix10!A13)</f>
         <v>0</v>
@@ -6585,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>SUM(matrix1:matrix10!A14)</f>
         <v>0</v>
@@ -6699,7 +6871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>SUM(matrix1:matrix10!A15)</f>
         <v>0</v>
@@ -6813,7 +6985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>SUM(matrix1:matrix10!A16)</f>
         <v>0</v>
@@ -6927,7 +7099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>SUM(matrix1:matrix10!A17)</f>
         <v>0</v>
@@ -7041,7 +7213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>SUM(matrix1:matrix10!A18)</f>
         <v>0</v>
@@ -7155,7 +7327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>SUM(matrix1:matrix10!A19)</f>
         <v>0</v>
@@ -7269,7 +7441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>SUM(matrix1:matrix10!A20)</f>
         <v>0</v>
@@ -7383,7 +7555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>SUM(matrix1:matrix10!A21)</f>
         <v>0</v>
@@ -7497,7 +7669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>SUM(matrix1:matrix10!A22)</f>
         <v>0</v>
@@ -7611,7 +7783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>SUM(matrix1:matrix10!A23)</f>
         <v>0</v>
@@ -7725,7 +7897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>SUM(matrix1:matrix10!A24)</f>
         <v>0</v>
@@ -7839,7 +8011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>SUM(matrix1:matrix10!A25)</f>
         <v>0</v>
@@ -7953,7 +8125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>SUM(matrix1:matrix10!A26)</f>
         <v>0</v>
@@ -8067,7 +8239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>SUM(matrix1:matrix10!A27)</f>
         <v>0</v>
@@ -8181,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>SUM(matrix1:matrix10!A28)</f>
         <v>0</v>
@@ -8308,12 +8480,12 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -8399,7 +8571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8485,7 +8657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -8571,7 +8743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -8657,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -8743,7 +8915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -8829,7 +9001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -8915,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -9001,7 +9173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -9087,7 +9259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -9173,7 +9345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -9259,7 +9431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -9345,7 +9517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -9431,7 +9603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -9517,7 +9689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -9603,7 +9775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -9689,7 +9861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -9775,7 +9947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -9861,7 +10033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -9947,7 +10119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -10033,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -10119,7 +10291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -10205,7 +10377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -10291,7 +10463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -10377,7 +10549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -10463,7 +10635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -10549,7 +10721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -10635,7 +10807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -10728,18 +10900,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF37439E-4EE7-4C95-B626-4D001A8BB674}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="AB31" sqref="AB31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -10825,7 +10997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10911,7 +11083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -10997,7 +11169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -11083,7 +11255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -11169,7 +11341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -11255,7 +11427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -11341,7 +11513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -11427,7 +11599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -11513,7 +11685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -11599,7 +11771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -11685,7 +11857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -11771,7 +11943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -11857,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -11943,7 +12115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -12029,7 +12201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -12115,7 +12287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -12201,7 +12373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -12287,7 +12459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -12373,7 +12545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -12459,7 +12631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -12545,7 +12717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -12631,7 +12803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -12717,7 +12889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -12803,7 +12975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -12889,7 +13061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -12972,6 +13144,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>
@@ -12982,18 +13326,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78C7E7C-6055-4881-889B-3BB7E45C22B6}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+      <selection activeCell="A26" sqref="A26:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -13079,7 +13423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -13165,7 +13509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -13251,7 +13595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -13337,7 +13681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -13423,7 +13767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -13509,7 +13853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -13595,7 +13939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -13681,7 +14025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -13767,7 +14111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -13853,7 +14197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -13939,7 +14283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -14025,7 +14369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -14111,7 +14455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -14197,7 +14541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -14283,7 +14627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -14369,7 +14713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -14455,7 +14799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -14541,7 +14885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -14627,7 +14971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -14713,7 +15057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -14799,7 +15143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -14885,7 +15229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -14971,7 +15315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -15057,7 +15401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -15143,7 +15487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -15226,6 +15570,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>
@@ -15236,18 +15752,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C457335-E6AD-479C-8BEA-A3815AAE1E64}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+      <selection activeCell="A26" sqref="A26:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -15333,7 +15849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -15419,7 +15935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -15505,7 +16021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -15591,7 +16107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -15677,7 +16193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -15763,7 +16279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -15849,7 +16365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -15935,7 +16451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -16021,7 +16537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -16107,7 +16623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -16193,7 +16709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -16279,7 +16795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -16365,7 +16881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -16451,7 +16967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -16537,7 +17053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -16623,7 +17139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -16709,7 +17225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -16795,7 +17311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -16881,7 +17397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -16967,7 +17483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -17053,7 +17569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -17139,7 +17655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -17225,7 +17741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -17311,7 +17827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -17397,7 +17913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -17480,6 +17996,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>
@@ -17490,18 +18178,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CED1D05-2AA1-4F1A-A057-F27747283F1F}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="A26" sqref="A26:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -17587,7 +18275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -17673,7 +18361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -17759,7 +18447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -17845,7 +18533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -17931,7 +18619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -18017,7 +18705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -18103,7 +18791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -18189,7 +18877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -18275,7 +18963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -18361,7 +19049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -18447,7 +19135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -18533,7 +19221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -18619,7 +19307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -18705,7 +19393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -18791,7 +19479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -18877,7 +19565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -18963,7 +19651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -19049,7 +19737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -19135,7 +19823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -19221,7 +19909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -19307,7 +19995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -19393,7 +20081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -19479,7 +20167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -19565,7 +20253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -19651,7 +20339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -19734,6 +20422,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>
@@ -19744,18 +20604,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4EFD2E-A8B2-407F-9172-A10A8DF065F1}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:X22"/>
+      <selection activeCell="A26" sqref="A26:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -19841,7 +20701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -19927,7 +20787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -20013,7 +20873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -20099,7 +20959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -20185,7 +21045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -20271,7 +21131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -20357,7 +21217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -20443,7 +21303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -20529,7 +21389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -20615,7 +21475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -20701,7 +21561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -20787,7 +21647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -20873,7 +21733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -20959,7 +21819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -21045,7 +21905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -21131,7 +21991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -21217,7 +22077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -21303,7 +22163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -21389,7 +22249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -21475,7 +22335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -21561,7 +22421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -21647,7 +22507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -21733,7 +22593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -21819,7 +22679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -21905,7 +22765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -21988,6 +22848,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>
@@ -21998,18 +23030,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9216B8-FFA2-4A6A-973F-A7929C0F1176}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+      <selection activeCell="A26" sqref="A26:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -22095,7 +23127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -22181,7 +23213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -22267,7 +23299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -22353,7 +23385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -22439,7 +23471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -22525,7 +23557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -22611,7 +23643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -22697,7 +23729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -22783,7 +23815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -22869,7 +23901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -22955,7 +23987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -23041,7 +24073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -23127,7 +24159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -23213,7 +24245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -23299,7 +24331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -23385,7 +24417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -23471,7 +24503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -23557,7 +24589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -23643,7 +24675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -23729,7 +24761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -23815,7 +24847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -23901,7 +24933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -23987,7 +25019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -24073,7 +25105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -24159,7 +25191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -24242,6 +25274,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>
@@ -24252,18 +25456,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBD6D3D-41BD-4BE0-8741-F7D9742C2EF9}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="A26" sqref="A26:AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="28" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -24349,7 +25553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -24435,7 +25639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -24521,7 +25725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -24607,7 +25811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -24693,7 +25897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -24779,7 +25983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -24865,7 +26069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -24951,7 +26155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -25037,7 +26241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -25123,7 +26327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -25209,7 +26413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -25295,7 +26499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -25381,7 +26585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -25467,7 +26671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -25553,7 +26757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -25639,7 +26843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -25725,7 +26929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -25811,7 +27015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -25897,7 +27101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -25983,7 +27187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -26069,7 +27273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -26155,7 +27359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -26241,7 +27445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -26327,7 +27531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -26413,7 +27617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -26496,6 +27700,178 @@
         <v>0</v>
       </c>
       <c r="AB26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0</v>
       </c>
     </row>

</xml_diff>